<commit_message>
corrected the URL in the Testcase file
</commit_message>
<xml_diff>
--- a/API TEST CASE FOR Petstore.xlsx
+++ b/API TEST CASE FOR Petstore.xlsx
@@ -52,7 +52,7 @@
   </si>
   <si>
     <t>URL -&gt; https://petstore.swagger.io/v2
-pet/6</t>
+pet/237</t>
   </si>
   <si>
     <t>1. 200 OK
@@ -77,7 +77,7 @@
   </si>
   <si>
     <t>URL -&gt; https://petstore.swagger.io/v2
-pet/6    Text: OK</t>
+pet/237    Text: OK</t>
   </si>
   <si>
     <t>1. 200 OK
@@ -99,7 +99,7 @@
   </si>
   <si>
     <t>URL -&gt; https://petstore.swagger.io/v2
-pet/6                                              ID no:279</t>
+pet/237                                              ID no:237</t>
   </si>
   <si>
     <t>1. 200 OK
@@ -134,7 +134,7 @@
   </si>
   <si>
     <t>URL -&gt; https://petstore.swagger.io/v2
-pet/6                                              Name: &lt;categoryname&gt;</t>
+pet/237                                              Name: &lt;categoryname&gt;</t>
   </si>
   <si>
     <t>1. 200 OK
@@ -151,7 +151,7 @@
   </si>
   <si>
     <t>URL -&gt; https://petstore.swagger.io/v2
-pet/6                                             value : Name</t>
+pet/237                                             value : Name</t>
   </si>
   <si>
     <t>1. 200 OK
@@ -168,7 +168,7 @@
   </si>
   <si>
     <t>URL -&gt; https://petstore.swagger.io/v2
-pet/6                                             value: status</t>
+pet/237                                             value: status</t>
   </si>
   <si>
     <t>200 OK was returned &amp; Body  response showing pending was observed</t>

</xml_diff>